<commit_message>
verify company vote card class created
</commit_message>
<xml_diff>
--- a/TestAutomationFramework/src/test/resources/testdata.xlsx
+++ b/TestAutomationFramework/src/test/resources/testdata.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6531D7B-D0BF-430C-8E18-E3B5486A4BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{79DD0951-3E87-486B-B35D-15823E6D2B4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="368" windowWidth="19425" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CountryFilter" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>country</t>
   </si>
@@ -46,9 +47,6 @@
   </si>
   <si>
     <t>chrome-headless</t>
-  </si>
-  <si>
-    <t>BelgiumTest</t>
   </si>
 </sst>
 </file>
@@ -434,7 +432,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -456,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>